<commit_message>
Added MS Excel sheet to prevent further error
</commit_message>
<xml_diff>
--- a/Global/Excel/SkillDesc.xlsx
+++ b/Global/Excel/SkillDesc.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1E633611-D942-4176-8E20-FD544BF3B83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E40BAF-86D2-497D-89B2-B6E3FBFED0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SkillDesc" sheetId="1" r:id="rId1"/>
@@ -4894,7 +4894,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5842,7 +5842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DJ222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -5854,99 +5854,118 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="54.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.25" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="73.25" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="38.75" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="62.375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="53" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="52" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="63.75" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="102.875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="36.75" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="16" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="52.75" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="70" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="68.375" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="68.375" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="11" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="1"/>
+    <col min="14" max="14" width="54.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9" style="1"/>
+    <col min="30" max="30" width="18.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9" style="1"/>
+    <col min="35" max="35" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="73.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="38.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9" style="1"/>
+    <col min="40" max="40" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="62.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="53" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9" style="1"/>
+    <col min="45" max="45" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="52" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="63.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9" style="1"/>
+    <col min="50" max="50" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="102.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="36.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9" style="1"/>
+    <col min="55" max="55" width="16.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="24.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="9" style="1"/>
+    <col min="60" max="60" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="52.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="9" style="1"/>
+    <col min="65" max="65" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="70" style="1" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="26.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="9" style="1"/>
+    <col min="70" max="70" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="68.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="9" style="1"/>
+    <col min="75" max="75" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="68.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="9" style="1"/>
+    <col min="80" max="80" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9" style="1"/>
+    <col min="85" max="85" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="9" style="1"/>
+    <col min="90" max="90" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="9" style="1"/>
+    <col min="95" max="95" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="21.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="9" style="1"/>
+    <col min="100" max="100" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="21.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="9" style="1"/>
+    <col min="105" max="105" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="19.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="9" style="1"/>
+    <col min="110" max="110" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="115" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:114" x14ac:dyDescent="0.2">
@@ -26211,5 +26230,6 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Skill - Barbarian - Leap: - Baseline minimum distance increased - Speed of the leap motion increased by 75% (may not work in 1.13) - Leap now has a minimum jump height and duration
Skill - Barbarian - Leap Attack:
- Speed of the leap motion increased by 75% (may not work in 1.13)
- Leap attack now has a minimum jump height and duration
- Damage baseline increased from 100% to 200%
- Attack Rating baseline increased from 50% to 100%
- Attack Rating per level increased from 15% to 20%

Skill - Barbarian - Berserk:
- Shout synergy replaced with Battle Orders

Skill - Barbarian - Double Throw:
- Added damage bonus with 16% baseline and 8% damage increase per level

Skill - Barbarian - Frenzy:
- Increased Stamina synergy added: +0.4 Seconds per Level
</commit_message>
<xml_diff>
--- a/Global/Excel/SkillDesc.xlsx
+++ b/Global/Excel/SkillDesc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E40BAF-86D2-497D-89B2-B6E3FBFED0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB64153-9BBE-4271-A786-980C56D35CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="1623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="1624">
   <si>
     <t>skilldesc</t>
   </si>
@@ -4889,6 +4889,10 @@
   </si>
   <si>
     <t>Runeword22</t>
+  </si>
+  <si>
+    <t>skillname149</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -5846,10 +5850,10 @@
   <dimension ref="A1:DJ222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BU125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="CL154" sqref="CL154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -19788,7 +19792,7 @@
         <v>175</v>
       </c>
       <c r="CL154" s="1" t="s">
-        <v>1086</v>
+        <v>1623</v>
       </c>
       <c r="CM154" s="1" t="s">
         <v>227</v>

</xml_diff>

<commit_message>
Updated Frenzy skill description
</commit_message>
<xml_diff>
--- a/Global/Excel/SkillDesc.xlsx
+++ b/Global/Excel/SkillDesc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB64153-9BBE-4271-A786-980C56D35CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C0159E-4C38-4BF1-A387-BB9CB5D56521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="1624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6605" uniqueCount="1625">
   <si>
     <t>skilldesc</t>
   </si>
@@ -4893,6 +4893,9 @@
   <si>
     <t>skillname149</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>par7+skill('Increased Stamina'.blvl)*10</t>
   </si>
 </sst>
 </file>
@@ -5850,10 +5853,10 @@
   <dimension ref="A1:DJ222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BU125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BD125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CL154" sqref="CL154"/>
+      <selection pane="bottomRight" activeCell="BJ149" sqref="BJ149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -19299,7 +19302,7 @@
         <v>189</v>
       </c>
       <c r="BJ149" s="1" t="s">
-        <v>297</v>
+        <v>1624</v>
       </c>
       <c r="BL149" s="1" t="s">
         <v>116</v>

</xml_diff>